<commit_message>
refactor: Borrar segmentaciones de primas de movilidad
</commit_message>
<xml_diff>
--- a/data/segmentacion_movilidad.xlsx
+++ b/data/segmentacion_movilidad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10329"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB4F2FD-55BB-4C4A-8400-B3856CA9E4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F68B4E-89A8-2B4D-B451-D6EED4E9126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29140" windowHeight="16160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29140" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
   <si>
     <t>codigo_op</t>
   </si>
@@ -568,8 +568,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -786,133 +786,90 @@
   <sheetPr codeName="Hoja2">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.15">
-      <c r="G17" s="1"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4330,8 +4287,8 @@
   </sheetPr>
   <dimension ref="A1:B401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fix: Corregir cuadre primas en segmentacion movilidad
</commit_message>
<xml_diff>
--- a/data/segmentacion_movilidad.xlsx
+++ b/data/segmentacion_movilidad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8E3C8F-A24E-984E-95A6-6C07AC2CD060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20DCCA-6F2F-774B-BE47-C22314B72AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29140" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29140" windowHeight="16160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="26">
   <si>
     <t>codigo_op</t>
   </si>
@@ -1000,7 +1000,7 @@
   </sheetPr>
   <dimension ref="A1:G397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -11008,39 +11008,32 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>